<commit_message>
Planeacion: EDT(project)...se adecuó al ciclo de vida en V, Presupuesto...se modificó la duraccion de las tareas para hacer una estimacion del costo del proyecto, GANTT...se cambió el flujo de tareas y su duracion
</commit_message>
<xml_diff>
--- a/Documentacion/2 Planeacion/Presupuesto.xlsx
+++ b/Documentacion/2 Planeacion/Presupuesto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIOVANNI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MEPPP\Documentacion\2 Planeacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{73B1C773-C080-46EE-82FA-A76A26354DE3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{472472E2-0EA9-416E-BA7E-99CFB1C03E46}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{1B7383BE-45CC-4E2F-A610-FCE863D259E3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="93">
   <si>
     <t>Sueldo del proyecto</t>
   </si>
@@ -124,12 +124,6 @@
     <t>Bolígrafo, Hojas de papel</t>
   </si>
   <si>
-    <t>Programador 1, Programador 2, Programador 3, Programador 4</t>
-  </si>
-  <si>
-    <t>Programador 1, Programador 2, Programador 3, Programador 3</t>
-  </si>
-  <si>
     <t>Lider de proyecto</t>
   </si>
   <si>
@@ -196,9 +190,6 @@
     <t>2.6 Plan de comunicación</t>
   </si>
   <si>
-    <t>2.7 Póliticas de calidad</t>
-  </si>
-  <si>
     <t>3.1 Análisis de provedores</t>
   </si>
   <si>
@@ -257,6 +248,63 @@
   </si>
   <si>
     <t xml:space="preserve">8.2 Acta de cierre del proyecto </t>
+  </si>
+  <si>
+    <t>5.3.1 Index</t>
+  </si>
+  <si>
+    <t>5.3.2 Invernadero</t>
+  </si>
+  <si>
+    <t>5.3.3 Campañas</t>
+  </si>
+  <si>
+    <t>5.3.4 Socios</t>
+  </si>
+  <si>
+    <t>5.3.5 Comentarios</t>
+  </si>
+  <si>
+    <t>5.3.6 FAQs</t>
+  </si>
+  <si>
+    <t>5.3.7 ¿Quiénes somos?</t>
+  </si>
+  <si>
+    <t>5.3.8 Login/Registro</t>
+  </si>
+  <si>
+    <t>5.3.9 Perfil</t>
+  </si>
+  <si>
+    <t>5.4.1 Adopciones</t>
+  </si>
+  <si>
+    <t>5.4.2 Invernaredo</t>
+  </si>
+  <si>
+    <t>5.4.3 Campañas</t>
+  </si>
+  <si>
+    <t>5.4.4 Comentarios</t>
+  </si>
+  <si>
+    <t>5.4.5 FAQs</t>
+  </si>
+  <si>
+    <t>5.4.6 Usuarios</t>
+  </si>
+  <si>
+    <t>5.4.7 ¿Quiénes somos?</t>
+  </si>
+  <si>
+    <t>6.3 Pruebas de validación</t>
+  </si>
+  <si>
+    <t>Programador 2</t>
+  </si>
+  <si>
+    <t>Programador 3</t>
   </si>
 </sst>
 </file>
@@ -335,7 +383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +435,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFAEAAAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,7 +514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -588,6 +642,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -599,8 +659,8 @@
   <colors>
     <mruColors>
       <color rgb="FFFF5050"/>
+      <color rgb="FF99FF99"/>
       <color rgb="FF66FF66"/>
-      <color rgb="FF99FF99"/>
       <color rgb="FFAEAAAA"/>
     </mruColors>
   </colors>
@@ -912,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C6BBF4-9154-4808-B240-AA9E19E178E7}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,8 +1025,8 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G3" s="35">
-        <f>SUM(G4,G6,G14,G20,G25,G30,G33,G37)</f>
-        <v>139119.21734575226</v>
+        <f>SUM(G4,G6,G13,G19,G24,G45,G49,G53)</f>
+        <v>87396.074006496478</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -981,10 +1041,10 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5" s="20">
         <f>LOOKUP(C5,Sueldos!B3,Sueldos!G3)</f>
@@ -1010,17 +1070,17 @@
       <c r="E6" s="10"/>
       <c r="F6" s="31"/>
       <c r="G6" s="36">
-        <f>SUM(G7:G13)</f>
-        <v>6996.2750000000005</v>
+        <f>SUM(G7:G12)</f>
+        <v>6585.0375000000004</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="20">
         <f>LOOKUP(C7,Sueldos!B3,Sueldos!G3)*8</f>
@@ -1040,10 +1100,10 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="20">
         <f>LOOKUP(C8,Sueldos!B3,Sueldos!G3)*8</f>
@@ -1056,17 +1116,17 @@
         <v>18</v>
       </c>
       <c r="G8" s="33">
-        <f t="shared" ref="G8:G13" si="0">D8+F8</f>
+        <f t="shared" ref="G8:G12" si="0">D8+F8</f>
         <v>1538.95</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" s="20">
         <f>LOOKUP(C9,Sueldos!B3,Sueldos!G3)*2</f>
@@ -1086,10 +1146,10 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" s="20">
         <f>LOOKUP(C10,Sueldos!B3,Sueldos!G3)*2</f>
@@ -1109,10 +1169,10 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="20">
         <f>LOOKUP(C11,Sueldos!B3,Sueldos!G3)*8</f>
@@ -1132,10 +1192,10 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" s="20">
         <f>LOOKUP(C12,Sueldos!B3,Sueldos!G3)*6</f>
@@ -1153,43 +1213,43 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="20">
-        <f>LOOKUP(C13,Sueldos!B3,Sueldos!G3)*2</f>
-        <v>380.23750000000001</v>
-      </c>
-      <c r="E13" s="11" t="s">
+      <c r="A13" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="36">
+        <f>SUM(G14:G18)</f>
+        <v>6046.9344002963535</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="20">
+        <f>LOOKUP(C14,Sueldos!B4,Sueldos!G4)*16</f>
+        <v>2358.280072990698</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="31">
-        <v>31</v>
-      </c>
-      <c r="G13" s="33">
-        <f t="shared" si="0"/>
-        <v>411.23750000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="36">
-        <f>SUM(G15:G19)</f>
-        <v>4278.2243455533298</v>
+      <c r="F14" s="31">
+        <v>31</v>
+      </c>
+      <c r="G14" s="33">
+        <f>D14+F14</f>
+        <v>2389.280072990698</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>5</v>
@@ -1199,43 +1259,43 @@
         <v>589.57001824767451</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F15" s="31">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="G15" s="33">
-        <f>D15+F15</f>
-        <v>620.57001824767451</v>
+        <f t="shared" ref="G15:G18" si="1">D15+F15</f>
+        <v>593.57001824767451</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="20">
-        <f>LOOKUP(C16,Sueldos!B4,Sueldos!G4)*4</f>
-        <v>589.57001824767451</v>
+        <f>LOOKUP(C16,Sueldos!B4,Sueldos!G4)*2</f>
+        <v>294.78500912383726</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F16" s="31">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G16" s="33">
-        <f t="shared" ref="G16:G19" si="1">D16+F16</f>
-        <v>593.57001824767451</v>
+        <f t="shared" si="1"/>
+        <v>312.78500912383726</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>5</v>
@@ -1245,131 +1305,131 @@
         <v>294.78500912383726</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F17" s="31">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G17" s="33">
         <f t="shared" si="1"/>
-        <v>312.78500912383726</v>
+        <v>329.78500912383726</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18" s="20">
-        <f>LOOKUP(C18,Sueldos!B4,Sueldos!G4)*2</f>
-        <v>294.78500912383726</v>
+        <f>LOOKUP(C18,Sueldos!B5,Sueldos!G5)*16</f>
+        <v>2399.5142908103066</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F18" s="31">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G18" s="33">
         <f t="shared" si="1"/>
-        <v>329.78500912383726</v>
+        <v>2421.5142908103066</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="17" t="s">
+      <c r="A19" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="36">
+        <f>SUM(G20:G23)</f>
+        <v>7283.5428724309204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="20">
-        <f>LOOKUP(C19,Sueldos!B5,Sueldos!G5)*16</f>
-        <v>2399.5142908103066</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="31">
-        <v>22</v>
-      </c>
-      <c r="G19" s="33">
-        <f t="shared" si="1"/>
-        <v>2421.5142908103066</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="36">
-        <f>SUM(G21:G24)</f>
-        <v>7283.5428724309204</v>
+      <c r="D20" s="20">
+        <f>LOOKUP(C20,Sueldos!B5,Sueldos!G5)*8</f>
+        <v>1199.7571454051533</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="31">
+        <v>18</v>
+      </c>
+      <c r="G20" s="32">
+        <f>D20+F20</f>
+        <v>1217.7571454051533</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="20">
-        <f>LOOKUP(C21,Sueldos!B5,Sueldos!G5)*8</f>
-        <v>1199.7571454051533</v>
+        <f>LOOKUP(C21,Sueldos!B5,Sueldos!G5)*20</f>
+        <v>2999.3928635128832</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F21" s="31">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G21" s="32">
-        <f>D21+F21</f>
-        <v>1217.7571454051533</v>
+        <f t="shared" ref="G21:G23" si="2">D21+F21</f>
+        <v>3030.3928635128832</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="20">
-        <f>LOOKUP(C22,Sueldos!B5,Sueldos!G5)*20</f>
-        <v>2999.3928635128832</v>
+        <f>LOOKUP(C22,Sueldos!B5,Sueldos!G5)*4</f>
+        <v>599.87857270257666</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F22" s="31">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G22" s="32">
-        <f t="shared" ref="G22:G24" si="2">D22+F22</f>
-        <v>3030.3928635128832</v>
+        <f t="shared" si="2"/>
+        <v>617.87857270257666</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="20">
-        <f>LOOKUP(C23,Sueldos!B5,Sueldos!G5)*4</f>
-        <v>599.87857270257666</v>
+        <f>LOOKUP(C23,Sueldos!B5,Sueldos!G5)*16</f>
+        <v>2399.5142908103066</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>26</v>
@@ -1379,50 +1439,50 @@
       </c>
       <c r="G23" s="32">
         <f t="shared" si="2"/>
-        <v>617.87857270257666</v>
+        <v>2417.5142908103066</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="20">
-        <f>LOOKUP(C24,Sueldos!B5,Sueldos!G5)*16</f>
-        <v>2399.5142908103066</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="31">
-        <v>18</v>
-      </c>
-      <c r="G24" s="32">
-        <f t="shared" si="2"/>
-        <v>2417.5142908103066</v>
+      <c r="A24" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="36">
+        <f>SUM(G25:G26,G28:G36,G38:G44)</f>
+        <v>52877.711747111949</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="36">
-        <f>SUM(G26:G29)</f>
-        <v>107315.60455505858</v>
+      <c r="A25" s="6"/>
+      <c r="B25" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="20">
+        <f>LOOKUP(C25,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="31">
+        <v>31</v>
+      </c>
+      <c r="G25" s="32">
+        <f>D25+F25</f>
+        <v>2583.1810608347282</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D26" s="20">
         <f>LOOKUP(C26,Sueldos!B6,Sueldos!G6)*16</f>
@@ -1435,44 +1495,35 @@
         <v>31</v>
       </c>
       <c r="G26" s="32">
-        <f>D26+F26</f>
+        <f t="shared" ref="G26:G37" si="3">D26+F26</f>
         <v>2583.1810608347282</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
-      <c r="B27" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="20">
-        <f>LOOKUP(C27,Sueldos!B6,Sueldos!G6)*16</f>
-        <v>2552.1810608347282</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="31">
-        <v>31</v>
-      </c>
-      <c r="G27" s="32">
-        <f t="shared" ref="G27:G29" si="3">D27+F27</f>
-        <v>2583.1810608347282</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="36">
+        <f>SUM(G28:G36)</f>
+        <v>25800.810608347285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="9" t="s">
-        <v>68</v>
+      <c r="B28" s="50" t="s">
+        <v>74</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="D28" s="20">
-        <f>LOOKUP(C28,Sueldos!B6,Sueldos!G6)*4*80</f>
-        <v>51043.621216694562</v>
+        <f>LOOKUP(C28,Sueldos!B6,Sueldos!G6)*24</f>
+        <v>3828.2715912520925</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>27</v>
@@ -1481,21 +1532,21 @@
         <v>31</v>
       </c>
       <c r="G28" s="32">
-        <f t="shared" si="3"/>
-        <v>51074.621216694562</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <f>D28+F28</f>
+        <v>3859.2715912520925</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="9" t="s">
-        <v>69</v>
+      <c r="B29" s="50" t="s">
+        <v>75</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="D29" s="20">
-        <f>LOOKUP(C29,Sueldos!B6,Sueldos!G6)*4*80</f>
-        <v>51043.621216694562</v>
+        <f>LOOKUP(C29,Sueldos!B6,Sueldos!G6)*24</f>
+        <v>3828.2715912520925</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>27</v>
@@ -1504,32 +1555,44 @@
         <v>31</v>
       </c>
       <c r="G29" s="32">
-        <f t="shared" si="3"/>
-        <v>51074.621216694562</v>
+        <f>D29+F29</f>
+        <v>3859.2715912520925</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="36">
-        <f>SUM(G31:G32)</f>
-        <v>7365.6316988173312</v>
+      <c r="A30" s="6"/>
+      <c r="B30" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="20">
+        <f>LOOKUP(C30,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="31">
+        <v>31</v>
+      </c>
+      <c r="G30" s="32">
+        <f>D30+F30</f>
+        <v>2583.1810608347282</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>8</v>
+      <c r="B31" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="D31" s="20">
-        <f>LOOKUP(C31,Sueldos!B7,Sueldos!G7)*24</f>
-        <v>3130.1278709217136</v>
+        <f>LOOKUP(C31,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>27</v>
@@ -1538,21 +1601,21 @@
         <v>31</v>
       </c>
       <c r="G31" s="32">
-        <f>D31+F31</f>
-        <v>3161.1278709217136</v>
+        <f t="shared" ref="G29:G36" si="4">D31+F31</f>
+        <v>2583.1810608347282</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>8</v>
+      <c r="B32" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="D32" s="20">
-        <f>LOOKUP(C32,Sueldos!B7,Sueldos!G7)*32</f>
-        <v>4173.5038278956181</v>
+        <f>LOOKUP(C32,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>27</v>
@@ -1561,33 +1624,44 @@
         <v>31</v>
       </c>
       <c r="G32" s="32">
-        <f>D32+F32</f>
-        <v>4204.5038278956181</v>
+        <f t="shared" si="4"/>
+        <v>2583.1810608347282</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="36">
-        <f>SUM(G34:G36)</f>
-        <v>4849.3451238921061</v>
+      <c r="A33" s="6"/>
+      <c r="B33" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="20">
+        <f>LOOKUP(C33,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="31">
+        <v>31</v>
+      </c>
+      <c r="G33" s="32">
+        <f t="shared" si="4"/>
+        <v>2583.1810608347282</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>6</v>
+      <c r="B34" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="D34" s="20">
-        <f>LOOKUP(C34,Sueldos!B5,Sueldos!G5)*8</f>
-        <v>1199.7571454051533</v>
+        <f>LOOKUP(C34,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>27</v>
@@ -1596,21 +1670,21 @@
         <v>31</v>
       </c>
       <c r="G34" s="32">
-        <f>D34+F34</f>
-        <v>1230.7571454051533</v>
+        <f t="shared" si="4"/>
+        <v>2583.1810608347282</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
-      <c r="B35" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>8</v>
+      <c r="B35" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="D35" s="20">
-        <f>LOOKUP(C35,Sueldos!B7,Sueldos!G7)*4</f>
-        <v>521.68797848695226</v>
+        <f>LOOKUP(C35,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>27</v>
@@ -1619,88 +1693,425 @@
         <v>31</v>
       </c>
       <c r="G35" s="32">
-        <f t="shared" ref="G35:G36" si="4">D35+F35</f>
-        <v>552.68797848695226</v>
+        <f t="shared" si="4"/>
+        <v>2583.1810608347282</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>34</v>
+      <c r="B36" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="D36" s="20">
-        <f>LOOKUP(C5,Sueldos!B3,Sueldos!G3)*16</f>
-        <v>3041.9</v>
+        <f>LOOKUP(C36,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F36" s="31">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G36" s="32">
         <f t="shared" si="4"/>
-        <v>3065.9</v>
+        <v>2583.1810608347282</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="18"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="20"/>
       <c r="E37" s="11"/>
       <c r="F37" s="31"/>
       <c r="G37" s="36">
-        <f>SUM(G38:G39)</f>
-        <v>808.47500000000002</v>
+        <f>SUM(G38:G44)</f>
+        <v>21910.539017095191</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
-      <c r="B38" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="18" t="s">
+      <c r="B38" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D38" s="20">
+        <f>LOOKUP(C38,Sueldos!B6,Sueldos!G6)*24</f>
+        <v>3828.2715912520925</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="31">
+        <v>31</v>
+      </c>
+      <c r="G38" s="32">
+        <f>D38+F38</f>
+        <v>3859.2715912520925</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="20">
+        <f>LOOKUP(C39,Sueldos!B6,Sueldos!G6)*24</f>
+        <v>3828.2715912520925</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="31">
+        <v>31</v>
+      </c>
+      <c r="G39" s="32">
+        <f t="shared" ref="G39:G44" si="5">D39+F39</f>
+        <v>3859.2715912520925</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="20">
+        <f>LOOKUP(C40,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="31">
+        <v>31</v>
+      </c>
+      <c r="G40" s="32">
+        <f t="shared" si="5"/>
+        <v>2583.1810608347282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="20">
+        <f>LOOKUP(C41,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" s="31">
+        <v>31</v>
+      </c>
+      <c r="G41" s="32">
+        <f t="shared" si="5"/>
+        <v>2583.1810608347282</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="20">
+        <f>LOOKUP(C42,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" s="31">
+        <v>31</v>
+      </c>
+      <c r="G42" s="32">
+        <f t="shared" si="5"/>
+        <v>2583.1810608347282</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="20">
+        <f>LOOKUP(C43,Sueldos!B6,Sueldos!G6)*24</f>
+        <v>3828.2715912520925</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" s="31">
+        <v>31</v>
+      </c>
+      <c r="G43" s="32">
+        <f t="shared" si="5"/>
+        <v>3859.2715912520925</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="20">
+        <f>LOOKUP(C44,Sueldos!B6,Sueldos!G6)*16</f>
+        <v>2552.1810608347282</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F44" s="31">
+        <v>31</v>
+      </c>
+      <c r="G44" s="32">
+        <f t="shared" si="5"/>
+        <v>2583.1810608347282</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="36">
+        <f>SUM(G46:G48)</f>
+        <v>9483.3836127651412</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="20">
+        <f>LOOKUP(C46,Sueldos!B7,Sueldos!G7)*24</f>
+        <v>3130.1278709217136</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="31">
+        <v>31</v>
+      </c>
+      <c r="G46" s="32">
+        <f>D46+F46</f>
+        <v>3161.1278709217136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="20">
+        <f>LOOKUP(C47,Sueldos!B7,Sueldos!G7)*32</f>
+        <v>4173.5038278956181</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F47" s="31">
+        <v>31</v>
+      </c>
+      <c r="G47" s="32">
+        <f>D47+F47</f>
+        <v>4204.5038278956181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="20">
+        <f>LOOKUP(C48,Sueldos!B7,Sueldos!G7)*16</f>
+        <v>2086.751913947809</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" s="31">
+        <v>31</v>
+      </c>
+      <c r="G48" s="32">
+        <f>D48+F48</f>
+        <v>2117.751913947809</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="18"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="36">
+        <f>SUM(G50:G52)</f>
+        <v>4088.8701238921058</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="20">
+        <f>LOOKUP(C50,Sueldos!B5,Sueldos!G5)*8</f>
+        <v>1199.7571454051533</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F50" s="31">
+        <v>31</v>
+      </c>
+      <c r="G50" s="32">
+        <f>D50+F50</f>
+        <v>1230.7571454051533</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="20">
+        <f>LOOKUP(C51,Sueldos!B7,Sueldos!G7)*4</f>
+        <v>521.68797848695226</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F51" s="31">
+        <v>31</v>
+      </c>
+      <c r="G51" s="32">
+        <f t="shared" ref="G51:G52" si="6">D51+F51</f>
+        <v>552.68797848695226</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+      <c r="B52" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="20">
+        <f>LOOKUP(C5,Sueldos!B3,Sueldos!G3)*12</f>
+        <v>2281.4250000000002</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F52" s="31">
+        <v>24</v>
+      </c>
+      <c r="G52" s="32">
+        <f t="shared" si="6"/>
+        <v>2305.4250000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="36">
+        <f>SUM(G54:G55)</f>
+        <v>808.47500000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="20">
         <f>LOOKUP(C5,Sueldos!B3,Sueldos!G3)*2</f>
         <v>380.23750000000001</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E54" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F38" s="31">
+      <c r="F54" s="31">
         <v>24</v>
       </c>
-      <c r="G38" s="32">
-        <f>D38+F38</f>
+      <c r="G54" s="32">
+        <f>D54+F54</f>
         <v>404.23750000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="20">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
+      <c r="B55" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="20">
         <f>LOOKUP(C5,Sueldos!B3,Sueldos!G3)*2</f>
         <v>380.23750000000001</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E55" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F39" s="31">
+      <c r="F55" s="31">
         <v>24</v>
       </c>
-      <c r="G39" s="32">
-        <f>D39+F39</f>
+      <c r="G55" s="32">
+        <f>D55+F55</f>
         <v>404.23750000000001</v>
       </c>
     </row>
@@ -1710,6 +2121,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D43" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1717,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45750D1-9947-4085-83DD-C22782B01263}">
   <dimension ref="B2:J38"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G10"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,7 +2163,7 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="41">
         <f>(C15*C12)/C15</f>
@@ -1959,7 +2373,7 @@
       <c r="C14" s="46"/>
       <c r="D14" s="5"/>
       <c r="E14" s="45" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F14" s="45"/>
       <c r="G14" s="45"/>
@@ -1967,14 +2381,14 @@
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15" s="40">
         <v>36443</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="48" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F15" s="49"/>
       <c r="G15" s="27">
@@ -1991,7 +2405,7 @@
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="48" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F16" s="49"/>
       <c r="G16" s="27">
@@ -2008,7 +2422,7 @@
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="48" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F17" s="49"/>
       <c r="G17" s="27">
@@ -2025,7 +2439,7 @@
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="48" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F18" s="49"/>
       <c r="G18" s="27">
@@ -2042,7 +2456,7 @@
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="48" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F19" s="49"/>
       <c r="G19" s="27">
@@ -2059,7 +2473,7 @@
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="48" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F20" s="49"/>
       <c r="G20" s="27">
@@ -2075,7 +2489,7 @@
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F21" s="49"/>
       <c r="G21" s="27">

</xml_diff>